<commit_message>
Added changes to display Response Text for Cancellast of Preauth response.
</commit_message>
<xml_diff>
--- a/Automation/static/XLS/card_data_sanity - Copy.xlsx
+++ b/Automation/static/XLS/card_data_sanity - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="292" firstSheet="1" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" tabRatio="292" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -9956,7 +9956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -12525,7 +12525,7 @@
   <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12768,8 +12768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>

</xml_diff>